<commit_message>
Added a flat tf value and dynamic threshold to the impored algorithm, seems to be a win in most cases
</commit_message>
<xml_diff>
--- a/hw3_precision_recall.xlsx
+++ b/hw3_precision_recall.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aharon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aharon\IdeaProjects\ir\hw3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -360,7 +360,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G3" sqref="E3:G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -408,13 +408,13 @@
         <v>0.33333333999999998</v>
       </c>
       <c r="E3">
-        <v>0.55555560000000004</v>
+        <v>0.66666669999999995</v>
       </c>
       <c r="F3">
-        <v>0.71428572999999995</v>
+        <v>0.85714287</v>
       </c>
       <c r="G3">
-        <v>0.31250002999999998</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -428,13 +428,13 @@
         <v>0.15384613999999999</v>
       </c>
       <c r="E4">
-        <v>5.2631579999999997E-2</v>
+        <v>0.22222222</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>4.9999996999999997E-2</v>
+        <v>0.18181818999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -448,13 +448,13 @@
         <v>5.8823532999999997E-2</v>
       </c>
       <c r="E5">
-        <v>2.8571428999999999E-2</v>
+        <v>5.2631579999999997E-2</v>
       </c>
       <c r="F5">
         <v>0.25</v>
       </c>
       <c r="G5">
-        <v>2.5641026000000001E-2</v>
+        <v>4.3478259999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -468,13 +468,13 @@
         <v>2.8571429999999998E-2</v>
       </c>
       <c r="E6">
-        <v>2.6315789999999999E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
         <v>0.2</v>
       </c>
       <c r="G6">
-        <v>2.3255814E-2</v>
+        <v>6.6666669999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -488,13 +488,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.22222222</v>
+        <v>7.1428574999999994E-2</v>
       </c>
       <c r="F7">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0.14285713</v>
+        <v>5.2631579999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -508,13 +508,13 @@
         <v>0.34782610000000003</v>
       </c>
       <c r="E8">
-        <v>0.32142857000000002</v>
+        <v>0.58333330000000005</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.77777779999999996</v>
       </c>
       <c r="G8">
-        <v>0.24324324999999999</v>
+        <v>0.3333333</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -528,13 +528,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2.4390242999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>2.3255814E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -551,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0.33333333999999998</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -568,13 +568,13 @@
         <v>0.27272728000000002</v>
       </c>
       <c r="E11">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="G11">
-        <v>0.33333333999999998</v>
+        <v>0.3846154</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -588,13 +588,13 @@
         <v>0.42857142999999998</v>
       </c>
       <c r="E12">
-        <v>0.26086956</v>
+        <v>0.75</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0.20689656000000001</v>
+        <v>0.42857142999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -608,13 +608,13 @@
         <v>0.15384613999999999</v>
       </c>
       <c r="E13">
-        <v>4.8780485999999998E-2</v>
+        <v>9.0909089999999998E-2</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G13">
-        <v>4.6511627999999999E-2</v>
+        <v>7.6923069999999996E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -631,10 +631,10 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0.14285714999999999</v>
+        <v>0.57142859999999995</v>
       </c>
       <c r="G14">
-        <v>0.125</v>
+        <v>0.36363636999999999</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -648,13 +648,13 @@
         <v>0.18181818999999999</v>
       </c>
       <c r="E15">
-        <v>8.108108E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0.66666669999999995</v>
       </c>
       <c r="G15">
-        <v>7.4999999999999997E-2</v>
+        <v>0.18181818999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -668,13 +668,13 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>2.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>2.4390245000000001E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -688,13 +688,13 @@
         <v>0.40000004</v>
       </c>
       <c r="E17">
-        <v>0.19047620000000001</v>
+        <v>0.8</v>
       </c>
       <c r="F17">
         <v>0.8</v>
       </c>
       <c r="G17">
-        <v>0.15384616000000001</v>
+        <v>0.40000004</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -708,13 +708,13 @@
         <v>0.33333333999999998</v>
       </c>
       <c r="E18">
-        <v>8.108108E-2</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0.66666669999999995</v>
       </c>
       <c r="G18">
-        <v>7.4999999999999997E-2</v>
+        <v>0.22222223999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -728,13 +728,13 @@
         <v>0.5</v>
       </c>
       <c r="E19">
-        <v>5.1282052000000002E-2</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
-        <v>4.8780490000000003E-2</v>
+        <v>0.22222223999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -748,13 +748,13 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>5.8823529999999999E-2</v>
+        <v>5.2631579999999997E-2</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>5.5555552000000001E-2</v>
+        <v>4.9999996999999997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -768,13 +768,13 @@
         <v>0.20000002</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="F21">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G21">
-        <v>0.16666665999999999</v>
+        <v>0.20000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -808,13 +808,13 @@
         <v>0.33333333999999998</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F23">
         <v>0.5</v>
       </c>
       <c r="G23">
-        <v>0.33333333999999998</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -828,13 +828,13 @@
         <v>0.2</v>
       </c>
       <c r="E24">
-        <v>4.8780485999999998E-2</v>
+        <v>0.2</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>4.6511627999999999E-2</v>
+        <v>0.16666665999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -868,13 +868,13 @@
         <v>0.5</v>
       </c>
       <c r="E26">
-        <v>3.125E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>3.0303031000000001E-2</v>
+        <v>0.33333333999999998</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -928,13 +928,13 @@
         <v>0.25</v>
       </c>
       <c r="E29">
-        <v>5.8823529999999999E-2</v>
+        <v>8.3333335999999994E-2</v>
       </c>
       <c r="F29">
-        <v>0.66666669999999995</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="G29">
-        <v>5.4054054999999997E-2</v>
+        <v>6.6666669999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -948,13 +948,13 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>0.11111111</v>
+        <v>0.13333333999999999</v>
       </c>
       <c r="F30">
         <v>0.4</v>
       </c>
       <c r="G30">
-        <v>8.6956515999999998E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -991,10 +991,10 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G32">
-        <v>0.16666665999999999</v>
+        <v>0.28571429999999998</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1008,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.10714286000000001</v>
+        <v>0.05</v>
       </c>
       <c r="F33">
-        <v>0.42857142999999998</v>
+        <v>0.14285714999999999</v>
       </c>
       <c r="G33">
-        <v>8.5714289999999999E-2</v>
+        <v>3.7037037000000002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1028,13 +1028,13 @@
         <v>8.3333335999999994E-2</v>
       </c>
       <c r="E34">
-        <v>3.4482760000000001E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34">
-        <v>3.3333334999999999E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1068,13 +1068,13 @@
         <v>0.5</v>
       </c>
       <c r="E36">
-        <v>2.6315789999999999E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>2.5641026000000001E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1088,13 +1088,13 @@
         <v>0.25</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1171,10 +1171,10 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>0.11111111</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="G41">
-        <v>9.9999993999999995E-2</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1188,13 +1188,13 @@
         <v>0.38888887</v>
       </c>
       <c r="E42">
-        <v>0.26470589999999999</v>
+        <v>0.63636360000000003</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0.77777779999999996</v>
       </c>
       <c r="G42">
-        <v>0.20930234</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1208,13 +1208,13 @@
         <v>0.11111111999999999</v>
       </c>
       <c r="E43">
-        <v>0.13513512999999999</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="F43">
-        <v>0.83333330000000005</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="G43">
-        <v>0.116279066</v>
+        <v>0.15384616000000001</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1248,13 +1248,13 @@
         <v>0.33333333999999998</v>
       </c>
       <c r="E45">
-        <v>0.18181818999999999</v>
+        <v>0.66666669999999995</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45">
-        <v>0.15384613999999999</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1268,13 +1268,13 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.1</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46">
-        <v>9.0909089999999998E-2</v>
+        <v>0.22222223999999999</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1288,13 +1288,13 @@
         <v>0.14285714999999999</v>
       </c>
       <c r="E47">
-        <v>9.6774189999999996E-2</v>
+        <v>8.3333335999999994E-2</v>
       </c>
       <c r="F47">
         <v>0.6</v>
       </c>
       <c r="G47">
-        <v>8.3333329999999997E-2</v>
+        <v>7.3170739999999998E-2</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1308,13 +1308,13 @@
         <v>0.3</v>
       </c>
       <c r="E48">
-        <v>0.51851849999999999</v>
+        <v>0.75</v>
       </c>
       <c r="F48">
-        <v>0.77777779999999996</v>
+        <v>0.16666666999999999</v>
       </c>
       <c r="G48">
-        <v>0.31111109999999997</v>
+        <v>0.13636364000000001</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1328,13 +1328,13 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>0.13636364000000001</v>
+        <v>0.25</v>
       </c>
       <c r="F49">
-        <v>0.5</v>
+        <v>0.33333333999999998</v>
       </c>
       <c r="G49">
-        <v>0.107142866</v>
+        <v>0.14285713</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1348,13 +1348,13 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>6.25E-2</v>
+        <v>0.16666666999999999</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50">
-        <v>5.8823529999999999E-2</v>
+        <v>0.14285714999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1368,13 +1368,13 @@
         <v>0.35294115999999998</v>
       </c>
       <c r="E51">
-        <v>0.27586207000000001</v>
+        <v>0.8</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G51">
-        <v>0.2162162</v>
+        <v>0.30769232000000002</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1408,13 +1408,13 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>0.2</v>
+        <v>0.16666666999999999</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0.66666669999999995</v>
       </c>
       <c r="G53">
-        <v>0.16666665999999999</v>
+        <v>0.13333333999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,13 +1448,13 @@
         <v>0.5</v>
       </c>
       <c r="E55">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
         <v>0.4</v>
-      </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
-        <v>0.28571429999999998</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1468,13 +1468,13 @@
         <v>9.0909089999999998E-2</v>
       </c>
       <c r="E56">
-        <v>3.3333334999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1488,13 +1488,13 @@
         <v>0.3</v>
       </c>
       <c r="E57">
-        <v>0.33333333999999998</v>
+        <v>0.625</v>
       </c>
       <c r="F57">
-        <v>0.66666669999999995</v>
+        <v>0.41666666000000002</v>
       </c>
       <c r="G57">
-        <v>0.22222223999999999</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1528,13 +1528,13 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F59">
         <v>0.5</v>
       </c>
       <c r="G59">
-        <v>0.14285714999999999</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1548,13 +1548,13 @@
         <v>0.21428572000000001</v>
       </c>
       <c r="E60">
-        <v>0.27586207000000001</v>
+        <v>0.6</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G60">
-        <v>0.2162162</v>
+        <v>0.33333333999999998</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -1568,13 +1568,13 @@
         <v>0.14285714999999999</v>
       </c>
       <c r="E61">
-        <v>0.10526315999999999</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="F61">
         <v>1</v>
       </c>
       <c r="G61">
-        <v>9.5238100000000006E-2</v>
+        <v>0.22222223999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed basic indexer to use top 20 words as stop words
</commit_message>
<xml_diff>
--- a/hw3_precision_recall.xlsx
+++ b/hw3_precision_recall.xlsx
@@ -128,7 +128,7 @@
     <cellStyle name="טוב" xfId="1" builtinId="26"/>
     <cellStyle name="רע" xfId="2" builtinId="27"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -162,36 +162,6 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -505,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection sqref="A1:G61"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -600,13 +570,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7.6923080000000005E-2</v>
+        <v>4.3478259999999998E-2</v>
       </c>
       <c r="B5">
         <v>0.25</v>
       </c>
       <c r="C5">
-        <v>5.8823532999999997E-2</v>
+        <v>3.7037037000000002E-2</v>
       </c>
       <c r="E5" s="2">
         <v>5.5555555999999999E-2</v>
@@ -660,13 +630,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>0.57142859999999995</v>
+        <v>0.39130433999999997</v>
       </c>
       <c r="B8">
-        <v>0.88888889999999998</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0.34782610000000003</v>
+        <v>0.28125</v>
       </c>
       <c r="E8" s="1">
         <v>0.77777779999999996</v>
@@ -760,13 +730,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>0.22222222</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>0.18181818999999999</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0.15384613999999999</v>
       </c>
       <c r="E13" s="2">
         <v>0.125</v>
@@ -800,13 +770,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>0.25</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="B15">
         <v>0.66666669999999995</v>
       </c>
       <c r="C15">
-        <v>0.18181818999999999</v>
+        <v>0.2</v>
       </c>
       <c r="E15" s="1">
         <v>0.5</v>
@@ -940,13 +910,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>0</v>
+        <v>9.6153850000000006E-3</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>9.5238100000000006E-3</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -980,13 +950,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>0.25</v>
+        <v>0.28571429999999998</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0.2</v>
+        <v>0.22222223999999999</v>
       </c>
       <c r="E24">
         <v>0.16666666999999999</v>
@@ -1220,13 +1190,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1360,13 +1330,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>0.16666666999999999</v>
+        <v>0.23076922999999999</v>
       </c>
       <c r="B43">
-        <v>0.33333333999999998</v>
+        <v>0.5</v>
       </c>
       <c r="C43">
-        <v>0.11111111999999999</v>
+        <v>0.15789475</v>
       </c>
       <c r="E43" s="1">
         <v>0.5</v>
@@ -1460,13 +1430,13 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>0.75</v>
+        <v>0.69230769999999997</v>
       </c>
       <c r="B48">
         <v>0.5</v>
       </c>
       <c r="C48">
-        <v>0.3</v>
+        <v>0.29032257</v>
       </c>
       <c r="E48" s="2">
         <v>0.6</v>
@@ -1620,13 +1590,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>0.11111111</v>
+        <v>0.125</v>
       </c>
       <c r="B56">
         <v>0.5</v>
       </c>
       <c r="C56">
-        <v>9.0909089999999998E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E56" s="1">
         <v>0.2</v>
@@ -1700,13 +1670,13 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="B60">
         <v>0.375</v>
       </c>
       <c r="C60">
-        <v>0.21428572000000001</v>
+        <v>0.23076922999999999</v>
       </c>
       <c r="E60" s="1">
         <v>0.71428572999999995</v>
@@ -1740,7 +1710,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>$A$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>